<commit_message>
update bounding box strategy
</commit_message>
<xml_diff>
--- a/materials/joint_index.xlsx
+++ b/materials/joint_index.xlsx
@@ -125,11 +125,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>correction: parent index here in original implementation is 1 (neck), which seems wrong.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>the first column: annotation indexes for corresponding joints in mpi_inf_3dhp dataset (0-27, which in MATLAB are 1-28)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>modification: parent index here in original implementation is 1 (neck)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -543,7 +543,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -590,7 +590,7 @@
         <v>head</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -955,7 +955,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>